<commit_message>
resolve IG errors and upgrade to latest IG publisher version
</commit_message>
<xml_diff>
--- a/v0.7/StructureDefinition-Communication.xlsx
+++ b/v0.7/StructureDefinition-Communication.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="295">
   <si>
     <t>Property</t>
   </si>
@@ -99,7 +99,7 @@
     <t>Base Definition</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/StructureDefinition/DomainResource</t>
+    <t>http://hl7.org/fhir/StructureDefinition/Communication</t>
   </si>
   <si>
     <t>Abstract</t>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>A record of information transmitted from a sender to a receiver</t>
-  </si>
-  <si>
-    <t>DomainResource</t>
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
@@ -417,16 +414,6 @@
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
   </si>
   <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>DomainResource.extension</t>
   </si>
   <si>
@@ -450,51 +437,179 @@
     <t>DomainResource.modifierExtension</t>
   </si>
   <si>
-    <t>Communication.about</t>
+    <t>Communication.identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier
+</t>
+  </si>
+  <si>
+    <t>Unique identifier</t>
+  </si>
+  <si>
+    <t>Business identifiers assigned to this communication by the performer or other systems which remain constant as the resource is updated and propagates from server to server.</t>
+  </si>
+  <si>
+    <t>This is a business identifier, not a resource identifier (see [discussion](resource.html#identifiers)).  It is best practice for the identifier to only appear on a single resource instance, however business practices may occasionally dictate that multiple resource instances with the same identifier can exist - possibly even with different resource types.  For example, multiple Patient and a Person resource instance might share the same social insurance number.</t>
+  </si>
+  <si>
+    <t>Allows identification of the communication as it is known by various participating systems and in a way that remains consistent across servers.</t>
+  </si>
+  <si>
+    <t>Event.identifier</t>
+  </si>
+  <si>
+    <t>FiveWs.identifier</t>
+  </si>
+  <si>
+    <t>Communication.instantiatesCanonical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">canonical(PlanDefinition|ActivityDefinition|Measure|OperationDefinition|Questionnaire)
+</t>
+  </si>
+  <si>
+    <t>Instantiates FHIR protocol or definition</t>
+  </si>
+  <si>
+    <t>The URL pointing to a FHIR-defined protocol, guideline, orderset or other definition that is adhered to in whole or in part by this Communication.</t>
+  </si>
+  <si>
+    <t>Event.instantiatesCanonical</t>
+  </si>
+  <si>
+    <t>.outboundRelationship[typeCode=DEFN].target</t>
+  </si>
+  <si>
+    <t>Communication.instantiatesUri</t>
+  </si>
+  <si>
+    <t>Instantiates external protocol or definition</t>
+  </si>
+  <si>
+    <t>The URL pointing to an externally maintained protocol, guideline, orderset or other definition that is adhered to in whole or in part by this Communication.</t>
+  </si>
+  <si>
+    <t>This might be an HTML page, PDF, etc. or could just be a non-resolvable URI identifier.</t>
+  </si>
+  <si>
+    <t>Event.instantiatesUri</t>
+  </si>
+  <si>
+    <t>Communication.basedOn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fulfills
+</t>
   </si>
   <si>
     <t xml:space="preserve">Reference(Resource)
 </t>
   </si>
   <si>
-    <t>Resources that pertain to this communication</t>
-  </si>
-  <si>
-    <t>Other resources that pertain to this communication and to which this communication should be associated.</t>
-  </si>
-  <si>
-    <t>Don't use Communication.about element when a more specific element exists, such as basedOn or reasonReference.</t>
-  </si>
-  <si>
-    <t>FiveWs.context</t>
-  </si>
-  <si>
-    <t>Communication.basedOn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fulfills
+    <t>Request fulfilled by this communication</t>
+  </si>
+  <si>
+    <t>An order, proposal or plan fulfilled in whole or in part by this Communication.</t>
+  </si>
+  <si>
+    <t>This must point to some sort of a 'Request' resource, such as CarePlan, CommunicationRequest, ServiceRequest, MedicationRequest, etc.</t>
+  </si>
+  <si>
+    <t>Event.basedOn</t>
+  </si>
+  <si>
+    <t>Communication.partOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">container
 </t>
   </si>
   <si>
-    <t>Request fulfilled by this communication</t>
-  </si>
-  <si>
-    <t>An order, proposal or plan fulfilled in whole or in part by this Communication.</t>
-  </si>
-  <si>
-    <t>This must point to some sort of a 'Request' resource, such as CarePlan, CommunicationRequest, ServiceRequest, MedicationRequest, etc.</t>
-  </si>
-  <si>
-    <t>Event.basedOn</t>
-  </si>
-  <si>
-    <t>Communication.category</t>
+    <t>Part of this action</t>
+  </si>
+  <si>
+    <t>Part of this action.</t>
+  </si>
+  <si>
+    <t>Event.partOf</t>
+  </si>
+  <si>
+    <t>Communication.inResponseTo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Communication)
+</t>
+  </si>
+  <si>
+    <t>Reply to</t>
+  </si>
+  <si>
+    <t>Prior communication that this communication is in response to.</t>
+  </si>
+  <si>
+    <t>Communication.status</t>
+  </si>
+  <si>
+    <t>preparation | in-progress | not-done | on-hold | stopped | completed | entered-in-error | unknown</t>
+  </si>
+  <si>
+    <t>The status of the transmission.</t>
+  </si>
+  <si>
+    <t>This element is labeled as a modifier because the status contains the codes aborted and entered-in-error that mark the communication as not currently valid.</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>The status of the communication.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/event-status|4.0.1</t>
+  </si>
+  <si>
+    <t>Event.status</t>
+  </si>
+  <si>
+    <t>FiveWs.status</t>
+  </si>
+  <si>
+    <t>Communication.statusReason</t>
+  </si>
+  <si>
+    <t>Suspended Reason
+Cancelled Reason</t>
   </si>
   <si>
     <t xml:space="preserve">CodeableConcept
 </t>
   </si>
   <si>
+    <t>Reason for current status</t>
+  </si>
+  <si>
+    <t>Captures the reason for the current state of the Communication.</t>
+  </si>
+  <si>
+    <t>This is generally only used for "exception" statuses such as "not-done", "suspended" or "aborted". The reason for performing the event at all is captured in reasonCode, not here.</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes for the reason why a communication did not happen.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/communication-not-done-reason</t>
+  </si>
+  <si>
+    <t>Event.statusReason</t>
+  </si>
+  <si>
+    <t>Communication.category</t>
+  </si>
+  <si>
     <t>Message category</t>
   </si>
   <si>
@@ -504,9 +619,6 @@
     <t>There may be multiple axes of categorization and one communication may serve multiple purposes.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
     <t>Codes for general categories of communications such as alerts, instructions, etc.</t>
   </si>
   <si>
@@ -514,6 +626,101 @@
   </si>
   <si>
     <t>FiveWs.class</t>
+  </si>
+  <si>
+    <t>Communication.priority</t>
+  </si>
+  <si>
+    <t>routine | urgent | asap | stat</t>
+  </si>
+  <si>
+    <t>Characterizes how quickly the planned or in progress communication must be addressed. Includes concepts such as stat, urgent, routine.</t>
+  </si>
+  <si>
+    <t>Used to prioritize workflow (such as which communication to read first) when the communication is planned or in progress.</t>
+  </si>
+  <si>
+    <t>If missing, this communication should be treated with normal priority</t>
+  </si>
+  <si>
+    <t>Codes indicating the relative importance of a communication.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/request-priority|4.0.1</t>
+  </si>
+  <si>
+    <t>FiveWs.grade</t>
+  </si>
+  <si>
+    <t>Communication.medium</t>
+  </si>
+  <si>
+    <t>A channel of communication</t>
+  </si>
+  <si>
+    <t>A channel that was used for this communication (e.g. email, fax).</t>
+  </si>
+  <si>
+    <t>Codes for communication mediums such as phone, fax, email, in person, etc.</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/ValueSet/v3-ParticipationMode</t>
+  </si>
+  <si>
+    <t>Communication.subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Patient|Group)
+</t>
+  </si>
+  <si>
+    <t>Focus of message</t>
+  </si>
+  <si>
+    <t>The patient or group that was the focus of this communication.</t>
+  </si>
+  <si>
+    <t>Event.subject</t>
+  </si>
+  <si>
+    <t>FiveWs.subject</t>
+  </si>
+  <si>
+    <t>Communication.topic</t>
+  </si>
+  <si>
+    <t>Description of the purpose/content</t>
+  </si>
+  <si>
+    <t>Description of the purpose/content, similar to a subject line in an email.</t>
+  </si>
+  <si>
+    <t>Communication.topic.text can be used without any codings.</t>
+  </si>
+  <si>
+    <t>Codes describing the purpose or content of the communication.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/communication-topic</t>
+  </si>
+  <si>
+    <t>FiveWs.context</t>
+  </si>
+  <si>
+    <t>Communication.about</t>
+  </si>
+  <si>
+    <t>Resources that pertain to this communication</t>
+  </si>
+  <si>
+    <t>Other resources that pertain to this communication and to which this communication should be associated.</t>
+  </si>
+  <si>
+    <t>Don't use Communication.about element when a more specific element exists, such as basedOn or reasonReference.</t>
   </si>
   <si>
     <t>Communication.encounter</t>
@@ -535,91 +742,180 @@
     <t>Event.context</t>
   </si>
   <si>
-    <t>Communication.identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier
+    <t>Communication.sent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateTime
 </t>
   </si>
   <si>
-    <t>Unique identifier</t>
-  </si>
-  <si>
-    <t>Business identifiers assigned to this communication by the performer or other systems which remain constant as the resource is updated and propagates from server to server.</t>
-  </si>
-  <si>
-    <t>This is a business identifier, not a resource identifier (see [discussion](http://hl7.org/fhir/R4/resource.html#identifiers)).  It is best practice for the identifier to only appear on a single resource instance, however business practices may occasionally dictate that multiple resource instances with the same identifier can exist - possibly even with different resource types.  For example, multiple Patient and a Person resource instance might share the same social insurance number.</t>
-  </si>
-  <si>
-    <t>Allows identification of the communication as it is known by various participating systems and in a way that remains consistent across servers.</t>
-  </si>
-  <si>
-    <t>Event.identifier</t>
-  </si>
-  <si>
-    <t>FiveWs.identifier</t>
-  </si>
-  <si>
-    <t>Communication.inResponseTo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Communication)
+    <t>When sent</t>
+  </si>
+  <si>
+    <t>The time when this communication was sent.</t>
+  </si>
+  <si>
+    <t>Event.occurrence[x] {Invariant: maps to period.start}</t>
+  </si>
+  <si>
+    <t>FiveWs.done[x]</t>
+  </si>
+  <si>
+    <t>Communication.received</t>
+  </si>
+  <si>
+    <t>When received</t>
+  </si>
+  <si>
+    <t>The time when this communication arrived at the destination.</t>
+  </si>
+  <si>
+    <t>Event.occurrence[x] {Invariant: maps to period.end}</t>
+  </si>
+  <si>
+    <t>Communication.recipient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Device|Organization|Patient|Practitioner|PractitionerRole|RelatedPerson|Group|CareTeam|HealthcareService)
 </t>
   </si>
   <si>
-    <t>Reply to</t>
-  </si>
-  <si>
-    <t>Prior communication that this communication is in response to.</t>
-  </si>
-  <si>
-    <t>Communication.instantiatesCanonical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">canonical(PlanDefinition|ActivityDefinition|Measure|OperationDefinition|Questionnaire)
+    <t>Message recipient</t>
+  </si>
+  <si>
+    <t>The entity (e.g. person, organization, clinical information system, care team or device) which was the target of the communication. If receipts need to be tracked by an individual, a separate resource instance will need to be created for each recipient.  Multiple recipient communications are intended where either receipts are not tracked (e.g. a mass mail-out) or a receipt is captured in aggregate (all emails confirmed received by a particular time).</t>
+  </si>
+  <si>
+    <t>Event.performer.actor</t>
+  </si>
+  <si>
+    <t>FiveWs.actor</t>
+  </si>
+  <si>
+    <t>Communication.sender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Device|Organization|Patient|Practitioner|PractitionerRole|RelatedPerson|HealthcareService)
 </t>
   </si>
   <si>
-    <t>Instantiates FHIR protocol or definition</t>
-  </si>
-  <si>
-    <t>The URL pointing to a FHIR-defined protocol, guideline, orderset or other definition that is adhered to in whole or in part by this Communication.</t>
-  </si>
-  <si>
-    <t>Event.instantiatesCanonical</t>
-  </si>
-  <si>
-    <t>.outboundRelationship[typeCode=DEFN].target</t>
-  </si>
-  <si>
-    <t>Communication.instantiatesUri</t>
-  </si>
-  <si>
-    <t>Instantiates external protocol or definition</t>
-  </si>
-  <si>
-    <t>The URL pointing to an externally maintained protocol, guideline, orderset or other definition that is adhered to in whole or in part by this Communication.</t>
-  </si>
-  <si>
-    <t>This might be an HTML page, PDF, etc. or could just be a non-resolvable URI identifier.</t>
-  </si>
-  <si>
-    <t>Event.instantiatesUri</t>
-  </si>
-  <si>
-    <t>Communication.medium</t>
-  </si>
-  <si>
-    <t>A channel of communication</t>
-  </si>
-  <si>
-    <t>A channel that was used for this communication (e.g. email, fax).</t>
-  </si>
-  <si>
-    <t>Codes for communication mediums such as phone, fax, email, in person, etc.</t>
-  </si>
-  <si>
-    <t>http://terminology.hl7.org/ValueSet/v3-ParticipationMode</t>
+    <t>Message sender</t>
+  </si>
+  <si>
+    <t>The entity (e.g. person, organization, clinical information system, or device) which was the source of the communication.</t>
+  </si>
+  <si>
+    <t>Communication.reasonCode</t>
+  </si>
+  <si>
+    <t>Indication for message</t>
+  </si>
+  <si>
+    <t>The reason or justification for the communication.</t>
+  </si>
+  <si>
+    <t>Textual reasons can be captured using reasonCode.text.</t>
+  </si>
+  <si>
+    <t>Codes for describing reasons for the occurrence of a communication.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/clinical-findings</t>
+  </si>
+  <si>
+    <t>Event.reasonCode</t>
+  </si>
+  <si>
+    <t>FiveWs.why[x]</t>
+  </si>
+  <si>
+    <t>.reasonCode</t>
+  </si>
+  <si>
+    <t>Communication.reasonReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Condition|Observation|DiagnosticReport|DocumentReference)
+</t>
+  </si>
+  <si>
+    <t>Why was communication done?</t>
+  </si>
+  <si>
+    <t>Indicates another resource whose existence justifies this communication.</t>
+  </si>
+  <si>
+    <t>Event.reasonReference</t>
+  </si>
+  <si>
+    <t>.outboundRelationship[typeCode=RSON].target</t>
+  </si>
+  <si>
+    <t>Communication.payload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BackboneElement
+</t>
+  </si>
+  <si>
+    <t>Message payload</t>
+  </si>
+  <si>
+    <t>Text, attachment(s), or resource(s) that was communicated to the recipient.</t>
+  </si>
+  <si>
+    <t>Communication.payload.id</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Communication.payload.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>Communication.payload.modifierExtension</t>
+  </si>
+  <si>
+    <t>extensions
+user contentmodifiers</t>
+  </si>
+  <si>
+    <t>Extensions that cannot be ignored even if unrecognized</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+  </si>
+  <si>
+    <t>BackboneElement.modifierExtension</t>
+  </si>
+  <si>
+    <t>Communication.payload.content[x]</t>
+  </si>
+  <si>
+    <t>string
+AttachmentReference(Resource)</t>
+  </si>
+  <si>
+    <t>Message part content</t>
+  </si>
+  <si>
+    <t>A communicated content (or for multi-part communications, one portion of the communication).</t>
   </si>
   <si>
     <t>Communication.note</t>
@@ -636,274 +932,6 @@
   </si>
   <si>
     <t>Event.note</t>
-  </si>
-  <si>
-    <t>Communication.partOf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">container
-</t>
-  </si>
-  <si>
-    <t>Part of this action</t>
-  </si>
-  <si>
-    <t>Part of this action.</t>
-  </si>
-  <si>
-    <t>Event.partOf</t>
-  </si>
-  <si>
-    <t>Communication.payload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BackboneElement
-</t>
-  </si>
-  <si>
-    <t>Message payload</t>
-  </si>
-  <si>
-    <t>Text, attachment(s), or resource(s) that was communicated to the recipient.</t>
-  </si>
-  <si>
-    <t>Communication.payload.content[x]</t>
-  </si>
-  <si>
-    <t>string
-AttachmentReference(Resource)</t>
-  </si>
-  <si>
-    <t>Message part content</t>
-  </si>
-  <si>
-    <t>A communicated content (or for multi-part communications, one portion of the communication).</t>
-  </si>
-  <si>
-    <t>Communication.priority</t>
-  </si>
-  <si>
-    <t>routine | urgent | asap | stat</t>
-  </si>
-  <si>
-    <t>Characterizes how quickly the planned or in progress communication must be addressed. Includes concepts such as stat, urgent, routine.</t>
-  </si>
-  <si>
-    <t>Used to prioritize workflow (such as which communication to read first) when the communication is planned or in progress.</t>
-  </si>
-  <si>
-    <t>If missing, this communication should be treated with normal priority</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>Codes indicating the relative importance of a communication.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/request-priority|4.0.1</t>
-  </si>
-  <si>
-    <t>FiveWs.grade</t>
-  </si>
-  <si>
-    <t>Communication.reasonCode</t>
-  </si>
-  <si>
-    <t>Indication for message</t>
-  </si>
-  <si>
-    <t>The reason or justification for the communication.</t>
-  </si>
-  <si>
-    <t>Textual reasons can be captured using reasonCode.text.</t>
-  </si>
-  <si>
-    <t>Codes for describing reasons for the occurrence of a communication.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/clinical-findings</t>
-  </si>
-  <si>
-    <t>Event.reasonCode</t>
-  </si>
-  <si>
-    <t>FiveWs.why[x]</t>
-  </si>
-  <si>
-    <t>.reasonCode</t>
-  </si>
-  <si>
-    <t>Communication.reasonReference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Condition|Observation|DiagnosticReport|DocumentReference)
-</t>
-  </si>
-  <si>
-    <t>Why was communication done?</t>
-  </si>
-  <si>
-    <t>Indicates another resource whose existence justifies this communication.</t>
-  </si>
-  <si>
-    <t>Event.reasonReference</t>
-  </si>
-  <si>
-    <t>.outboundRelationship[typeCode=RSON].target</t>
-  </si>
-  <si>
-    <t>Communication.received</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dateTime
-</t>
-  </si>
-  <si>
-    <t>When received</t>
-  </si>
-  <si>
-    <t>The time when this communication arrived at the destination.</t>
-  </si>
-  <si>
-    <t>Event.occurrence[x] {Invariant: maps to period.end}</t>
-  </si>
-  <si>
-    <t>FiveWs.done[x]</t>
-  </si>
-  <si>
-    <t>Communication.recipient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Device|Organization|Patient|Practitioner|PractitionerRole|RelatedPerson|Group|CareTeam|HealthcareService)
-</t>
-  </si>
-  <si>
-    <t>Message recipient</t>
-  </si>
-  <si>
-    <t>The entity (e.g. person, organization, clinical information system, care team or device) which was the target of the communication. If receipts need to be tracked by an individual, a separate resource instance will need to be created for each recipient.  Multiple recipient communications are intended where either receipts are not tracked (e.g. a mass mail-out) or a receipt is captured in aggregate (all emails confirmed received by a particular time).</t>
-  </si>
-  <si>
-    <t>Event.performer.actor</t>
-  </si>
-  <si>
-    <t>FiveWs.actor</t>
-  </si>
-  <si>
-    <t>Communication.sender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Device|Organization|Patient|Practitioner|PractitionerRole|RelatedPerson|HealthcareService)
-</t>
-  </si>
-  <si>
-    <t>Message sender</t>
-  </si>
-  <si>
-    <t>The entity (e.g. person, organization, clinical information system, or device) which was the source of the communication.</t>
-  </si>
-  <si>
-    <t>Communication.sent</t>
-  </si>
-  <si>
-    <t>When sent</t>
-  </si>
-  <si>
-    <t>The time when this communication was sent.</t>
-  </si>
-  <si>
-    <t>Event.occurrence[x] {Invariant: maps to period.start}</t>
-  </si>
-  <si>
-    <t>Communication.status</t>
-  </si>
-  <si>
-    <t>preparation | in-progress | not-done | on-hold | stopped | completed | entered-in-error | unknown</t>
-  </si>
-  <si>
-    <t>The status of the transmission.</t>
-  </si>
-  <si>
-    <t>This element is labeled as a modifier because the status contains the codes aborted and entered-in-error that mark the communication as not currently valid.</t>
-  </si>
-  <si>
-    <t>The status of the communication.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/event-status|4.0.1</t>
-  </si>
-  <si>
-    <t>Event.status</t>
-  </si>
-  <si>
-    <t>FiveWs.status</t>
-  </si>
-  <si>
-    <t>Communication.statusReason</t>
-  </si>
-  <si>
-    <t>Suspended Reason
-Cancelled Reason</t>
-  </si>
-  <si>
-    <t>Reason for current status</t>
-  </si>
-  <si>
-    <t>Captures the reason for the current state of the Communication.</t>
-  </si>
-  <si>
-    <t>This is generally only used for "exception" statuses such as "not-done", "suspended" or "aborted". The reason for performing the event at all is captured in reasonCode, not here.</t>
-  </si>
-  <si>
-    <t>Codes for the reason why a communication did not happen.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/communication-not-done-reason</t>
-  </si>
-  <si>
-    <t>Event.statusReason</t>
-  </si>
-  <si>
-    <t>Communication.subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Patient|Group)
-</t>
-  </si>
-  <si>
-    <t>Focus of message</t>
-  </si>
-  <si>
-    <t>The patient or group that was the focus of this communication.</t>
-  </si>
-  <si>
-    <t>Event.subject</t>
-  </si>
-  <si>
-    <t>FiveWs.subject</t>
-  </si>
-  <si>
-    <t>Communication.topic</t>
-  </si>
-  <si>
-    <t>Description of the purpose/content</t>
-  </si>
-  <si>
-    <t>Description of the purpose/content, similar to a subject line in an email.</t>
-  </si>
-  <si>
-    <t>Communication.topic.text can be used without any codings.</t>
-  </si>
-  <si>
-    <t>Codes describing the purpose or content of the communication.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/communication-topic</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1226,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL34"/>
+  <dimension ref="A1:AL37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1207,7 +1235,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="34.6796875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="39.390625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
@@ -1234,7 +1262,7 @@
     <col min="25" max="25" width="57.484375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="34.6796875" customWidth="true" bestFit="true" hidden="true"/>
@@ -1445,7 +1473,7 @@
         <v>71</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="AF2" t="s" s="2">
         <v>72</v>
@@ -1457,21 +1485,21 @@
         <v>71</v>
       </c>
       <c r="AI2" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ2" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="AJ2" t="s" s="2">
+      <c r="AK2" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AL2" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AK2" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AL2" t="s" s="2">
-        <v>78</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -1482,28 +1510,28 @@
         <v>72</v>
       </c>
       <c r="F3" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="G3" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="I3" t="s" s="2">
+      <c r="J3" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="J3" t="s" s="2">
+      <c r="K3" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="K3" t="s" s="2">
+      <c r="L3" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="L3" t="s" s="2">
+      <c r="M3" t="s" s="2">
         <v>84</v>
-      </c>
-      <c r="M3" t="s" s="2">
-        <v>85</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" t="s" s="2">
@@ -1553,13 +1581,13 @@
         <v>71</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AF3" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>71</v>
@@ -1579,7 +1607,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
@@ -1590,25 +1618,25 @@
         <v>72</v>
       </c>
       <c r="F4" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="G4" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="H4" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="I4" t="s" s="2">
-        <v>81</v>
-      </c>
       <c r="J4" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="K4" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="K4" t="s" s="2">
+      <c r="L4" t="s" s="2">
         <v>89</v>
-      </c>
-      <c r="L4" t="s" s="2">
-        <v>90</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1659,19 +1687,19 @@
         <v>71</v>
       </c>
       <c r="AE4" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AF4" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AG4" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH4" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI4" t="s" s="2">
         <v>91</v>
-      </c>
-      <c r="AF4" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AG4" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH4" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AI4" t="s" s="2">
-        <v>92</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>71</v>
@@ -1685,7 +1713,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1696,28 +1724,28 @@
         <v>72</v>
       </c>
       <c r="F5" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="H5" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="G5" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>81</v>
-      </c>
       <c r="I5" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J5" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K5" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="K5" t="s" s="2">
+      <c r="L5" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="L5" t="s" s="2">
+      <c r="M5" t="s" s="2">
         <v>96</v>
-      </c>
-      <c r="M5" t="s" s="2">
-        <v>97</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -1767,19 +1795,19 @@
         <v>71</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ5" t="s" s="2">
         <v>71</v>
@@ -1793,7 +1821,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1804,7 +1832,7 @@
         <v>72</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>71</v>
@@ -1816,16 +1844,16 @@
         <v>71</v>
       </c>
       <c r="J6" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="K6" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="K6" t="s" s="2">
+      <c r="L6" t="s" s="2">
         <v>101</v>
       </c>
-      <c r="L6" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>102</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -1851,43 +1879,43 @@
         <v>71</v>
       </c>
       <c r="W6" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="X6" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="X6" t="s" s="2">
+      <c r="Y6" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="Y6" t="s" s="2">
+      <c r="Z6" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA6" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB6" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC6" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD6" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE6" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="Z6" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AA6" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AB6" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AC6" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>107</v>
-      </c>
       <c r="AF6" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>71</v>
@@ -1901,18 +1929,18 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
         <v>72</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s" s="2">
         <v>71</v>
@@ -1924,16 +1952,16 @@
         <v>71</v>
       </c>
       <c r="J7" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="K7" t="s" s="2">
         <v>110</v>
       </c>
-      <c r="K7" t="s" s="2">
+      <c r="L7" t="s" s="2">
         <v>111</v>
       </c>
-      <c r="L7" t="s" s="2">
+      <c r="M7" t="s" s="2">
         <v>112</v>
-      </c>
-      <c r="M7" t="s" s="2">
-        <v>113</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -1983,37 +2011,37 @@
         <v>71</v>
       </c>
       <c r="AE7" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="AF7" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AG7" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH7" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI7" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AK7" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AL7" t="s" s="2">
         <v>114</v>
-      </c>
-      <c r="AF7" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AG7" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH7" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AI7" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AK7" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AL7" t="s" s="2">
-        <v>115</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -2032,16 +2060,16 @@
         <v>71</v>
       </c>
       <c r="J8" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="K8" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="K8" t="s" s="2">
+      <c r="L8" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="L8" t="s" s="2">
+      <c r="M8" t="s" s="2">
         <v>120</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>121</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2091,7 +2119,7 @@
         <v>71</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>72</v>
@@ -2112,16 +2140,16 @@
         <v>71</v>
       </c>
       <c r="AL8" t="s" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -2140,16 +2168,16 @@
         <v>71</v>
       </c>
       <c r="J9" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>126</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>127</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="M9" t="s" s="2">
         <v>128</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>129</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2187,19 +2215,19 @@
         <v>71</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>130</v>
+        <v>71</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="AC9" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>72</v>
@@ -2211,7 +2239,7 @@
         <v>71</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>71</v>
@@ -2220,16 +2248,16 @@
         <v>71</v>
       </c>
       <c r="AL9" t="s" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -2242,25 +2270,25 @@
         <v>71</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>71</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O10" t="s" s="2">
         <v>71</v>
@@ -2297,19 +2325,19 @@
         <v>71</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>130</v>
+        <v>71</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="AC10" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>72</v>
@@ -2321,7 +2349,7 @@
         <v>71</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>71</v>
@@ -2330,12 +2358,12 @@
         <v>71</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -2355,21 +2383,23 @@
         <v>71</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="J11" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="K11" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="L11" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="M11" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="N11" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="K11" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="L11" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
         <v>71</v>
       </c>
@@ -2417,7 +2447,7 @@
         <v>71</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>72</v>
@@ -2429,13 +2459,13 @@
         <v>71</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AL11" t="s" s="2">
         <v>71</v>
@@ -2443,11 +2473,11 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>147</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -2463,20 +2493,18 @@
         <v>71</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>150</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
         <v>71</v>
@@ -2525,7 +2553,7 @@
         <v>71</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>72</v>
@@ -2537,21 +2565,21 @@
         <v>71</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>71</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2571,19 +2599,19 @@
         <v>71</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="J13" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K13" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="L13" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="M13" t="s" s="2">
         <v>153</v>
-      </c>
-      <c r="K13" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="L13" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>156</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -2609,13 +2637,13 @@
         <v>71</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>157</v>
+        <v>71</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>158</v>
+        <v>71</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>159</v>
+        <v>71</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>71</v>
@@ -2633,7 +2661,7 @@
         <v>71</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>72</v>
@@ -2645,53 +2673,53 @@
         <v>71</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>71</v>
+        <v>154</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>71</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>71</v>
+        <v>156</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
         <v>72</v>
       </c>
       <c r="F14" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="H14" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="I14" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="G14" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="H14" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="I14" t="s" s="2">
-        <v>81</v>
-      </c>
       <c r="J14" t="s" s="2">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -2741,25 +2769,25 @@
         <v>71</v>
       </c>
       <c r="AE14" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AF14" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AG14" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AH14" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI14" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
         <v>161</v>
       </c>
-      <c r="AF14" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AG14" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH14" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AI14" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AJ14" t="s" s="2">
-        <v>166</v>
-      </c>
       <c r="AK14" t="s" s="2">
-        <v>145</v>
+        <v>71</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>71</v>
@@ -2767,11 +2795,11 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>71</v>
+        <v>163</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -2787,23 +2815,19 @@
         <v>71</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>172</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>71</v>
       </c>
@@ -2851,7 +2875,7 @@
         <v>71</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>72</v>
@@ -2863,13 +2887,13 @@
         <v>71</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>174</v>
+        <v>71</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>71</v>
@@ -2877,7 +2901,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2900,13 +2924,13 @@
         <v>71</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2957,7 +2981,7 @@
         <v>71</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>72</v>
@@ -2969,7 +2993,7 @@
         <v>71</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ16" t="s" s="2">
         <v>71</v>
@@ -2983,7 +3007,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2991,30 +3015,32 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>71</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>180</v>
+        <v>99</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="M17" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="M17" t="s" s="2">
+        <v>174</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
         <v>71</v>
@@ -3039,13 +3065,13 @@
         <v>71</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>71</v>
+        <v>176</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>71</v>
+        <v>177</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>71</v>
@@ -3063,44 +3089,44 @@
         <v>71</v>
       </c>
       <c r="AE17" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="AF17" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="AF17" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AG17" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH17" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AI17" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AJ17" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="AK17" t="s" s="2">
-        <v>71</v>
-      </c>
       <c r="AL17" t="s" s="2">
-        <v>184</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>71</v>
+        <v>181</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
         <v>72</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>71</v>
@@ -3109,19 +3135,19 @@
         <v>71</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>94</v>
+        <v>182</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3147,13 +3173,13 @@
         <v>71</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>71</v>
+        <v>186</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>71</v>
+        <v>187</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>71</v>
+        <v>188</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>71</v>
@@ -3171,19 +3197,19 @@
         <v>71</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>189</v>
@@ -3192,7 +3218,7 @@
         <v>71</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>184</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19">
@@ -3220,7 +3246,7 @@
         <v>71</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="K19" t="s" s="2">
         <v>191</v>
@@ -3228,7 +3254,9 @@
       <c r="L19" t="s" s="2">
         <v>192</v>
       </c>
-      <c r="M19" s="2"/>
+      <c r="M19" t="s" s="2">
+        <v>193</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>71</v>
@@ -3253,13 +3281,13 @@
         <v>71</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>71</v>
@@ -3289,13 +3317,13 @@
         <v>71</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ19" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>71</v>
+        <v>196</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>71</v>
@@ -3303,7 +3331,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3314,7 +3342,7 @@
         <v>72</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>71</v>
@@ -3323,23 +3351,27 @@
         <v>71</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>196</v>
+        <v>99</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="M20" s="2"/>
+        <v>199</v>
+      </c>
+      <c r="M20" t="s" s="2">
+        <v>200</v>
+      </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="P20" s="2"/>
+      <c r="P20" t="s" s="2">
+        <v>201</v>
+      </c>
       <c r="Q20" t="s" s="2">
         <v>71</v>
       </c>
@@ -3359,13 +3391,13 @@
         <v>71</v>
       </c>
       <c r="W20" t="s" s="2">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="X20" t="s" s="2">
-        <v>71</v>
+        <v>202</v>
       </c>
       <c r="Y20" t="s" s="2">
-        <v>71</v>
+        <v>203</v>
       </c>
       <c r="Z20" t="s" s="2">
         <v>71</v>
@@ -3383,25 +3415,25 @@
         <v>71</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>199</v>
+        <v>71</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>71</v>
+        <v>204</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>71</v>
@@ -3409,11 +3441,11 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>201</v>
+        <v>71</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3429,16 +3461,16 @@
         <v>71</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>141</v>
+        <v>182</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3465,13 +3497,13 @@
         <v>71</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>71</v>
+        <v>186</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>71</v>
+        <v>208</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>71</v>
+        <v>209</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>71</v>
@@ -3489,7 +3521,7 @@
         <v>71</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>72</v>
@@ -3501,10 +3533,10 @@
         <v>71</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>204</v>
+        <v>71</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>71</v>
@@ -3515,18 +3547,18 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>71</v>
+        <v>211</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
         <v>72</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>71</v>
@@ -3535,16 +3567,16 @@
         <v>71</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3595,25 +3627,25 @@
         <v>71</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>71</v>
+        <v>215</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>71</v>
+        <v>216</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>71</v>
@@ -3621,7 +3653,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3629,10 +3661,10 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>71</v>
@@ -3644,15 +3676,17 @@
         <v>71</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="M23" s="2"/>
+        <v>219</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>71</v>
@@ -3677,13 +3711,13 @@
         <v>71</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>71</v>
+        <v>186</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>71</v>
+        <v>221</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>71</v>
+        <v>222</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>71</v>
@@ -3701,25 +3735,25 @@
         <v>71</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>71</v>
+        <v>223</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>71</v>
@@ -3727,7 +3761,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3738,7 +3772,7 @@
         <v>72</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>71</v>
@@ -3747,27 +3781,25 @@
         <v>71</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="P24" t="s" s="2">
-        <v>217</v>
-      </c>
+      <c r="P24" s="2"/>
       <c r="Q24" t="s" s="2">
         <v>71</v>
       </c>
@@ -3787,13 +3819,13 @@
         <v>71</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>218</v>
+        <v>71</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>219</v>
+        <v>71</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>220</v>
+        <v>71</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>71</v>
@@ -3811,25 +3843,25 @@
         <v>71</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>71</v>
@@ -3837,7 +3869,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3848,7 +3880,7 @@
         <v>72</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>71</v>
@@ -3857,19 +3889,19 @@
         <v>71</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>153</v>
+        <v>229</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -3895,13 +3927,13 @@
         <v>71</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>157</v>
+        <v>71</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>226</v>
+        <v>71</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>227</v>
+        <v>71</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>71</v>
@@ -3919,33 +3951,33 @@
         <v>71</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>230</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3956,7 +3988,7 @@
         <v>72</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>71</v>
@@ -3965,16 +3997,16 @@
         <v>71</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4025,33 +4057,33 @@
         <v>71</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AH26" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>236</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4062,7 +4094,7 @@
         <v>72</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>71</v>
@@ -4074,13 +4106,13 @@
         <v>71</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4131,25 +4163,25 @@
         <v>71</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>71</v>
@@ -4157,7 +4189,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4180,13 +4212,13 @@
         <v>71</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4237,7 +4269,7 @@
         <v>71</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>72</v>
@@ -4249,13 +4281,13 @@
         <v>71</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>71</v>
@@ -4263,7 +4295,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4274,7 +4306,7 @@
         <v>72</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>71</v>
@@ -4286,13 +4318,13 @@
         <v>71</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4343,25 +4375,25 @@
         <v>71</v>
       </c>
       <c r="AE29" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AK29" t="s" s="2">
         <v>249</v>
-      </c>
-      <c r="AF29" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>248</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>71</v>
@@ -4369,7 +4401,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4380,27 +4412,29 @@
         <v>72</v>
       </c>
       <c r="F30" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="G30" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="H30" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="I30" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="G30" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="H30" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="I30" t="s" s="2">
-        <v>71</v>
-      </c>
       <c r="J30" t="s" s="2">
-        <v>238</v>
+        <v>182</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="M30" s="2"/>
+        <v>256</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>257</v>
+      </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>71</v>
@@ -4425,13 +4459,13 @@
         <v>71</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>71</v>
+        <v>186</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>71</v>
+        <v>258</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>71</v>
+        <v>259</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>71</v>
@@ -4449,33 +4483,33 @@
         <v>71</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>71</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4483,32 +4517,30 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="F31" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="G31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="H31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="I31" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="F31" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="G31" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="H31" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="I31" t="s" s="2">
-        <v>81</v>
-      </c>
       <c r="J31" t="s" s="2">
-        <v>100</v>
+        <v>264</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>260</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>71</v>
@@ -4533,68 +4565,68 @@
         <v>71</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>218</v>
+        <v>71</v>
       </c>
       <c r="X31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Y31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Z31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE31" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="AF31" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AG31" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AH31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI31" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AK31" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="Y31" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="Z31" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AA31" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AB31" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AC31" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AD31" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AE31" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="AF31" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AG31" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH31" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AI31" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>264</v>
-      </c>
       <c r="AL31" t="s" s="2">
-        <v>71</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>266</v>
+        <v>71</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
         <v>72</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>71</v>
@@ -4603,20 +4635,18 @@
         <v>71</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>153</v>
+        <v>270</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>269</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>71</v>
@@ -4641,13 +4671,13 @@
         <v>71</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>157</v>
+        <v>71</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>270</v>
+        <v>71</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>271</v>
+        <v>71</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>71</v>
@@ -4665,22 +4695,22 @@
         <v>71</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>272</v>
+        <v>71</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>71</v>
@@ -4695,14 +4725,14 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>274</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>72</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>71</v>
@@ -4711,16 +4741,16 @@
         <v>71</v>
       </c>
       <c r="I33" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="J33" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="J33" t="s" s="2">
+      <c r="K33" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>275</v>
-      </c>
-      <c r="K33" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>277</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -4771,13 +4801,13 @@
         <v>71</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>71</v>
@@ -4786,29 +4816,29 @@
         <v>71</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>278</v>
+        <v>71</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>279</v>
+        <v>71</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>71</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>71</v>
+        <v>124</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>72</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>71</v>
@@ -4820,16 +4850,16 @@
         <v>71</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>281</v>
+        <v>126</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>283</v>
+        <v>128</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -4855,13 +4885,13 @@
         <v>71</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>157</v>
+        <v>71</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>284</v>
+        <v>71</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>285</v>
+        <v>71</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>71</v>
@@ -4885,21 +4915,343 @@
         <v>72</v>
       </c>
       <c r="AG34" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AH34" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI34" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AJ34" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AK34" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AL34" t="s" s="2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="F35" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="G35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="H35" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="AH34" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AI34" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="AL34" t="s" s="2">
+      <c r="I35" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J35" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="K35" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="L35" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="O35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="P35" s="2"/>
+      <c r="Q35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="R35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="S35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="T35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="U35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="V35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="W35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="X35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Y35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Z35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE35" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AL35" t="s" s="2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="F36" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="G36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="H36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="I36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="J36" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="K36" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="L36" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="P36" s="2"/>
+      <c r="Q36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="R36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="S36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="T36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="U36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="V36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="W36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="X36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Y36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Z36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE36" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="AF36" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AG36" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AK36" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AL36" t="s" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="F37" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="G37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="H37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="I37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="J37" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="K37" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="L37" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="P37" s="2"/>
+      <c r="Q37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="R37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="S37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="T37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="U37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="V37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="W37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="X37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Y37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Z37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE37" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="AF37" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AG37" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AH37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AI37" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AJ37" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>71</v>
       </c>
     </row>

</xml_diff>